<commit_message>
download of data p2
</commit_message>
<xml_diff>
--- a/files_creation/data/input/tickers.xlsx
+++ b/files_creation/data/input/tickers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33606\OneDrive - EDHEC\Desktop\Trading\SI\Stats_SI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33606\OneDrive - EDHEC\Desktop\Trading\SI\Stats_SI\files_creation\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C5A796-D422-479B-A20A-8CA5934A2EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF509B25-130B-48CD-9B27-145423EF5540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="2047">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="2046">
   <si>
     <t>Ticker</t>
   </si>
@@ -6155,9 +6155,6 @@
   </si>
   <si>
     <t>EVERSET</t>
-  </si>
-  <si>
-    <t>The BLOOMBERG PROFESSIONAL service, BLOOMBERG Data and BLOOMBERG Order Management Systems (the "Services") are owned and distributed locally by Bloomberg Finance L.P. ("BFLP") and its subsidiaries in all jurisdictions other than Argentina, Bermuda, China, India, Japan and Korea (the "BLP Countries"). BFLP is a wholly-owned subsidiary of Bloomberg L.P. ("BLP"). BLP provides BFLP with all global marketing and operational support and service for the Services and distributes the Services either directly or through a non-BFLP subsidiary in the BLP Countries. The Services include electronic trading and order-routing services, which are available only to sophisticated institutional investors and only where necessary legal clearances have been obtained. BFLP, BLP and their affiliates do not provide investment advice or guarantee the accuracy of prices or information in the Services. Nothing on the Services shall constitute an offering of financial instruments by BFLP, BLP or their affiliates. BLOOMBERG, BLOOMBERG PROFESSIONAL, BLOOMBERG MARKET, BLOOMBERG NEWS, BLOOMBERG ANYWHERE, BLOOMBERG TRADEBOOK, BLOOMBERG BONDTRADER, BLOOMBERG TELEVISION, BLOOMBERG RADIO, BLOOMBERG PRESS and BLOOMBERG.COM are trademarks and service marks of BFLP, a Delaware limited partnership, or its subsidiaries.</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -6311,7 +6308,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="28"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="28" applyAlignment="1">
@@ -6323,9 +6320,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="21">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -6674,8 +6668,8 @@
   </sheetPr>
   <dimension ref="A1:H1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A994" workbookViewId="0">
+      <selection activeCell="B1021" sqref="B1021"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -6750,7 +6744,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="12.75">
@@ -14873,16 +14867,15 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="1025" spans="1:2" ht="60" customHeight="1">
-      <c r="A1025" s="6" t="s">
-        <v>2045</v>
-      </c>
-      <c r="B1025" s="6"/>
+    <row r="1024" spans="1:2">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+    </row>
+    <row r="1025" spans="1:2">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1025:B1025"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>